<commit_message>
Some Drug Tweet Updates
Some more updates on the illicit drug tweets.
</commit_message>
<xml_diff>
--- a/Library for Illegal Online Activity.xlsx
+++ b/Library for Illegal Online Activity.xlsx
@@ -1264,7 +1264,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1448,7 +1448,7 @@
       <c r="C8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="7" t="s">

</xml_diff>